<commit_message>
Update workflow; fixed up data cleaning and prep report, working on fixing up analysis report
</commit_message>
<xml_diff>
--- a/codebooks/CSEC_Colombia_codebook.xlsx
+++ b/codebooks/CSEC_Colombia_codebook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2025_Colombia_CSEC\codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC7D3023-DCE8-458A-9737-F820D41A74C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135F6DD3-529F-4A16-8A83-7A37128F09DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13920" yWindow="0" windowWidth="14940" windowHeight="15585" xr2:uid="{90244CBB-F4EA-4ADF-B7F8-E6030CEF41FB}"/>
+    <workbookView xWindow="19275" yWindow="0" windowWidth="9630" windowHeight="15585" xr2:uid="{90244CBB-F4EA-4ADF-B7F8-E6030CEF41FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="366">
   <si>
     <t>Variable</t>
   </si>
@@ -1122,13 +1122,43 @@
     <t>Q503</t>
   </si>
   <si>
-    <t>Q4</t>
-  </si>
-  <si>
-    <t>Q406</t>
-  </si>
-  <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Independent Q.</t>
+  </si>
+  <si>
+    <t>Missing Status</t>
+  </si>
+  <si>
+    <t>Dependent on H19A</t>
+  </si>
+  <si>
+    <t>Dependent on selection and Q2&lt;18</t>
+  </si>
+  <si>
+    <t>Dependent on Q19</t>
+  </si>
+  <si>
+    <t>Dependent on Q29</t>
+  </si>
+  <si>
+    <t>Dependent on Q50, Q55, &amp; Q58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dependent on Q2&gt;=13 &amp; Q2 &lt;= 17 </t>
+  </si>
+  <si>
+    <t>Dependent on Q407</t>
+  </si>
+  <si>
+    <t>Dependent on Q1208</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -1186,27 +1216,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="11">
     <dxf>
-      <font>
-        <b/>
-      </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1231,18 +1279,6 @@
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1257,16 +1293,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3698636C-93CE-4425-935C-334B86A7B96E}" name="Table1" displayName="Table1" ref="A1:G123" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:G123" xr:uid="{3698636C-93CE-4425-935C-334B86A7B96E}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{2730ECEE-3C09-4BF5-890B-8860A9CFBE29}" name="Variable" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{1B48FA0F-CEB7-4E19-9CD2-A2270A8AEDC4}" name="VariableLabel" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{7642A26E-88CB-48B5-AECC-1FFA7324F1DD}" name="DataType" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{9DD7BF96-4287-49C0-901C-E4519D6003DE}" name="Questionnaire" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{BA0A682C-F3BF-499B-95BC-EB5277AFCFED}" name="RawNationalVar" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{1BA336CD-24B9-41F9-B139-898576B99FDF}" name="RawPriorityVar" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{9B023F9C-FAD5-4EB5-92F1-B039F8077C44}" name="Levels" dataDxfId="5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3698636C-93CE-4425-935C-334B86A7B96E}" name="Table1" displayName="Table1" ref="A1:I124" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:I124" xr:uid="{3698636C-93CE-4425-935C-334B86A7B96E}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{2730ECEE-3C09-4BF5-890B-8860A9CFBE29}" name="Variable" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{1B48FA0F-CEB7-4E19-9CD2-A2270A8AEDC4}" name="VariableLabel" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{7642A26E-88CB-48B5-AECC-1FFA7324F1DD}" name="DataType" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{9DD7BF96-4287-49C0-901C-E4519D6003DE}" name="Questionnaire" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{BA0A682C-F3BF-499B-95BC-EB5277AFCFED}" name="RawNationalVar" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{1BA336CD-24B9-41F9-B139-898576B99FDF}" name="RawPriorityVar" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{9B023F9C-FAD5-4EB5-92F1-B039F8077C44}" name="Levels" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{2315BC48-3D3F-48E3-9101-8995A5E0E366}" name="Missing Status" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{905ED3C1-4347-4C3A-B678-A272BEEDEC6B}" name="Column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1589,24 +1627,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70025C6-7774-44FB-9A43-8696DD932E81}">
-  <dimension ref="A1:G134"/>
+  <dimension ref="A1:I134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E104" sqref="E104:F116"/>
+    <sheetView tabSelected="1" topLeftCell="E12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="16" style="2" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" style="2" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1628,9 +1667,15 @@
       <c r="G1" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="H1" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1651,12 +1696,18 @@
       <c r="G2" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="H2" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1674,9 +1725,15 @@
       <c r="G3" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="H3" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1697,9 +1754,15 @@
       <c r="G4" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="H4" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1720,9 +1783,15 @@
       <c r="G5" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="H5" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1743,13 +1812,19 @@
       <c r="G6" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>14</v>
+      <c r="H6" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>41</v>
@@ -1758,44 +1833,56 @@
         <v>5</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>15</v>
+        <v>44</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>16</v>
+        <v>43</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>37</v>
@@ -1804,40 +1891,52 @@
         <v>5</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>17</v>
+      <c r="H9" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1858,9 +1957,15 @@
       <c r="G11" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="H11" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1881,8 +1986,12 @@
       <c r="G12" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>82</v>
       </c>
@@ -1901,8 +2010,12 @@
       <c r="F13" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>84</v>
       </c>
@@ -1919,10 +2032,14 @@
         <v>49</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>86</v>
       </c>
@@ -1938,8 +2055,12 @@
       <c r="F15" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>88</v>
       </c>
@@ -1953,10 +2074,14 @@
         <v>51</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>105</v>
       </c>
@@ -1972,8 +2097,14 @@
       <c r="F17" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H17" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>107</v>
       </c>
@@ -1989,8 +2120,12 @@
       <c r="F18" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H18" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>109</v>
       </c>
@@ -2006,8 +2141,12 @@
       <c r="F19" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H19" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>111</v>
       </c>
@@ -2023,8 +2162,12 @@
       <c r="F20" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H20" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>113</v>
       </c>
@@ -2040,8 +2183,14 @@
       <c r="F21" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H21" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -2057,8 +2206,12 @@
       <c r="F22" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H22" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>117</v>
       </c>
@@ -2074,8 +2227,12 @@
       <c r="F23" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H23" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>119</v>
       </c>
@@ -2089,10 +2246,16 @@
         <v>67</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>121</v>
       </c>
@@ -2108,8 +2271,14 @@
       <c r="F25" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H25" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>123</v>
       </c>
@@ -2125,8 +2294,14 @@
       <c r="F26" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H26" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>125</v>
       </c>
@@ -2142,8 +2317,12 @@
       <c r="F27" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H27" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>127</v>
       </c>
@@ -2159,8 +2338,12 @@
       <c r="F28" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H28" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>129</v>
       </c>
@@ -2176,8 +2359,14 @@
       <c r="F29" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H29" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>131</v>
       </c>
@@ -2193,8 +2382,12 @@
       <c r="F30" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H30" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>133</v>
       </c>
@@ -2210,8 +2403,14 @@
       <c r="F31" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H31" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>135</v>
       </c>
@@ -2227,8 +2426,12 @@
       <c r="F32" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H32" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>137</v>
       </c>
@@ -2244,8 +2447,14 @@
       <c r="F33" s="2" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H33" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>139</v>
       </c>
@@ -2261,8 +2470,14 @@
       <c r="F34" s="2" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H34" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>141</v>
       </c>
@@ -2278,8 +2493,14 @@
       <c r="F35" s="2" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H35" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>143</v>
       </c>
@@ -2295,8 +2516,14 @@
       <c r="F36" s="2" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H36" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>145</v>
       </c>
@@ -2312,8 +2539,14 @@
       <c r="F37" s="2" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H37" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>147</v>
       </c>
@@ -2329,8 +2562,14 @@
       <c r="F38" s="2" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H38" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>149</v>
       </c>
@@ -2346,8 +2585,14 @@
       <c r="F39" s="2" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H39" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>151</v>
       </c>
@@ -2363,8 +2608,14 @@
       <c r="F40" s="2" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H40" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>153</v>
       </c>
@@ -2380,8 +2631,12 @@
       <c r="F41" s="2" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H41" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I41" s="2"/>
+    </row>
+    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>155</v>
       </c>
@@ -2397,8 +2652,12 @@
       <c r="F42" s="2" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H42" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I42" s="2"/>
+    </row>
+    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>157</v>
       </c>
@@ -2414,8 +2673,12 @@
       <c r="F43" s="2" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H43" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I43" s="2"/>
+    </row>
+    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>159</v>
       </c>
@@ -2431,8 +2694,12 @@
       <c r="F44" s="2" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H44" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I44" s="2"/>
+    </row>
+    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>161</v>
       </c>
@@ -2448,8 +2715,12 @@
       <c r="F45" s="2" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H45" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I45" s="2"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>163</v>
       </c>
@@ -2465,8 +2736,12 @@
       <c r="F46" s="2" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H46" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I46" s="2"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>165</v>
       </c>
@@ -2482,8 +2757,12 @@
       <c r="F47" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H47" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I47" s="2"/>
+    </row>
+    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>167</v>
       </c>
@@ -2499,8 +2778,12 @@
       <c r="F48" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H48" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="I48" s="2"/>
+    </row>
+    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>169</v>
       </c>
@@ -2516,8 +2799,12 @@
       <c r="F49" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H49" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="I49" s="2"/>
+    </row>
+    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>171</v>
       </c>
@@ -2533,8 +2820,12 @@
       <c r="F50" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H50" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="I50" s="2"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>173</v>
       </c>
@@ -2550,8 +2841,12 @@
       <c r="F51" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H51" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I51" s="2"/>
+    </row>
+    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>175</v>
       </c>
@@ -2567,8 +2862,14 @@
       <c r="F52" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H52" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>177</v>
       </c>
@@ -2584,8 +2885,14 @@
       <c r="F53" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H53" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>179</v>
       </c>
@@ -2601,8 +2908,12 @@
       <c r="F54" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H54" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I54" s="2"/>
+    </row>
+    <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>181</v>
       </c>
@@ -2618,8 +2929,12 @@
       <c r="F55" s="2" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H55" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I55" s="2"/>
+    </row>
+    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>183</v>
       </c>
@@ -2635,8 +2950,12 @@
       <c r="F56" s="2" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H56" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I56" s="2"/>
+    </row>
+    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>185</v>
       </c>
@@ -2652,8 +2971,12 @@
       <c r="F57" s="2" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H57" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I57" s="2"/>
+    </row>
+    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>187</v>
       </c>
@@ -2669,8 +2992,12 @@
       <c r="F58" s="2" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H58" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I58" s="2"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>189</v>
       </c>
@@ -2686,8 +3013,12 @@
       <c r="F59" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H59" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I59" s="2"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>191</v>
       </c>
@@ -2703,8 +3034,12 @@
       <c r="F60" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H60" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I60" s="2"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>193</v>
       </c>
@@ -2720,8 +3055,12 @@
       <c r="F61" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H61" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I61" s="2"/>
+    </row>
+    <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>195</v>
       </c>
@@ -2737,8 +3076,14 @@
       <c r="F62" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H62" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>197</v>
       </c>
@@ -2754,8 +3099,12 @@
       <c r="F63" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H63" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I63" s="2"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>199</v>
       </c>
@@ -2771,8 +3120,12 @@
       <c r="F64" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H64" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I64" s="2"/>
+    </row>
+    <row r="65" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>201</v>
       </c>
@@ -2788,8 +3141,14 @@
       <c r="F65" s="2" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H65" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>203</v>
       </c>
@@ -2805,8 +3164,14 @@
       <c r="F66" s="2" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H66" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>205</v>
       </c>
@@ -2822,8 +3187,14 @@
       <c r="F67" s="2" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H67" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>207</v>
       </c>
@@ -2839,8 +3210,14 @@
       <c r="F68" s="2" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H68" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>209</v>
       </c>
@@ -2856,8 +3233,12 @@
       <c r="F69" s="2" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H69" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I69" s="2"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>211</v>
       </c>
@@ -2873,8 +3254,12 @@
       <c r="F70" s="2" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H70" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I70" s="2"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>213</v>
       </c>
@@ -2890,8 +3275,12 @@
       <c r="F71" s="2" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H71" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I71" s="2"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>215</v>
       </c>
@@ -2907,8 +3296,12 @@
       <c r="F72" s="2" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="H72" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I72" s="2"/>
+    </row>
+    <row r="73" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>217</v>
       </c>
@@ -2924,8 +3317,12 @@
       <c r="F73" s="2" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="H73" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I73" s="2"/>
+    </row>
+    <row r="74" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>219</v>
       </c>
@@ -2941,8 +3338,12 @@
       <c r="F74" s="2" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="H74" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I74" s="2"/>
+    </row>
+    <row r="75" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>221</v>
       </c>
@@ -2958,8 +3359,12 @@
       <c r="F75" s="2" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="H75" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I75" s="2"/>
+    </row>
+    <row r="76" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>223</v>
       </c>
@@ -2975,8 +3380,12 @@
       <c r="F76" s="2" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="H76" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I76" s="2"/>
+    </row>
+    <row r="77" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>225</v>
       </c>
@@ -2992,8 +3401,12 @@
       <c r="F77" s="2" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="H77" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I77" s="2"/>
+    </row>
+    <row r="78" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>227</v>
       </c>
@@ -3009,8 +3422,12 @@
       <c r="F78" s="2" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="H78" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I78" s="2"/>
+    </row>
+    <row r="79" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>229</v>
       </c>
@@ -3026,8 +3443,12 @@
       <c r="F79" s="2" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="H79" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I79" s="2"/>
+    </row>
+    <row r="80" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>231</v>
       </c>
@@ -3043,8 +3464,12 @@
       <c r="F80" s="2" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="H80" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I80" s="2"/>
+    </row>
+    <row r="81" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>233</v>
       </c>
@@ -3060,8 +3485,12 @@
       <c r="F81" s="2" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="H81" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I81" s="2"/>
+    </row>
+    <row r="82" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>235</v>
       </c>
@@ -3077,8 +3506,12 @@
       <c r="F82" s="2" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="H82" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I82" s="2"/>
+    </row>
+    <row r="83" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>237</v>
       </c>
@@ -3094,8 +3527,12 @@
       <c r="F83" s="2" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="H83" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I83" s="2"/>
+    </row>
+    <row r="84" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>239</v>
       </c>
@@ -3111,8 +3548,12 @@
       <c r="F84" s="2" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H84" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I84" s="2"/>
+    </row>
+    <row r="85" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>241</v>
       </c>
@@ -3128,8 +3569,14 @@
       <c r="F85" s="2" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H85" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>243</v>
       </c>
@@ -3145,8 +3592,14 @@
       <c r="F86" s="2" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H86" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>245</v>
       </c>
@@ -3162,8 +3615,14 @@
       <c r="F87" s="2" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H87" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>247</v>
       </c>
@@ -3179,8 +3638,14 @@
       <c r="F88" s="2" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H88" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="I88" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>249</v>
       </c>
@@ -3196,8 +3661,14 @@
       <c r="F89" s="2" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H89" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>251</v>
       </c>
@@ -3213,8 +3684,14 @@
       <c r="F90" s="2" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H90" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="I90" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>253</v>
       </c>
@@ -3230,8 +3707,12 @@
       <c r="F91" s="2" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H91" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I91" s="2"/>
+    </row>
+    <row r="92" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>255</v>
       </c>
@@ -3247,8 +3728,12 @@
       <c r="F92" s="2" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H92" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I92" s="2"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>257</v>
       </c>
@@ -3264,8 +3749,12 @@
       <c r="F93" s="2" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H93" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I93" s="2"/>
+    </row>
+    <row r="94" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>259</v>
       </c>
@@ -3281,8 +3770,12 @@
       <c r="F94" s="2" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H94" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I94" s="2"/>
+    </row>
+    <row r="95" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>261</v>
       </c>
@@ -3298,8 +3791,12 @@
       <c r="F95" s="2" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H95" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I95" s="2"/>
+    </row>
+    <row r="96" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>263</v>
       </c>
@@ -3315,8 +3812,12 @@
       <c r="F96" s="2" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H96" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I96" s="2"/>
+    </row>
+    <row r="97" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>265</v>
       </c>
@@ -3332,8 +3833,14 @@
       <c r="F97" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H97" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="I97" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>267</v>
       </c>
@@ -3349,8 +3856,14 @@
       <c r="F98" s="2" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H98" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I98" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>269</v>
       </c>
@@ -3366,8 +3879,14 @@
       <c r="F99" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H99" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I99" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>271</v>
       </c>
@@ -3383,8 +3902,14 @@
       <c r="F100" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H100" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I100" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>273</v>
       </c>
@@ -3400,8 +3925,14 @@
       <c r="F101" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H101" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I101" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>275</v>
       </c>
@@ -3417,8 +3948,12 @@
       <c r="F102" s="2" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H102" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I102" s="2"/>
+    </row>
+    <row r="103" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>277</v>
       </c>
@@ -3434,8 +3969,12 @@
       <c r="F103" s="2" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="H103" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I103" s="2"/>
+    </row>
+    <row r="104" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>279</v>
       </c>
@@ -3446,13 +3985,17 @@
         <v>48</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="I104" s="2"/>
+    </row>
+    <row r="105" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>281</v>
       </c>
@@ -3463,13 +4006,17 @@
         <v>48</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="I105" s="2"/>
+    </row>
+    <row r="106" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>283</v>
       </c>
@@ -3480,13 +4027,17 @@
         <v>48</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+      <c r="H106" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="I106" s="2"/>
+    </row>
+    <row r="107" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>285</v>
       </c>
@@ -3497,13 +4048,17 @@
         <v>48</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+      <c r="H107" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="I107" s="2"/>
+    </row>
+    <row r="108" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>287</v>
       </c>
@@ -3514,13 +4069,17 @@
         <v>48</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+      <c r="H108" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="I108" s="2"/>
+    </row>
+    <row r="109" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>289</v>
       </c>
@@ -3531,13 +4090,17 @@
         <v>48</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+      <c r="H109" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="I109" s="2"/>
+    </row>
+    <row r="110" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>291</v>
       </c>
@@ -3548,13 +4111,17 @@
         <v>48</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+      <c r="H110" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="I110" s="2"/>
+    </row>
+    <row r="111" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>293</v>
       </c>
@@ -3565,13 +4132,17 @@
         <v>48</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+      <c r="H111" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="I111" s="2"/>
+    </row>
+    <row r="112" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>295</v>
       </c>
@@ -3582,13 +4153,17 @@
         <v>48</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+      <c r="H112" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="I112" s="2"/>
+    </row>
+    <row r="113" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>297</v>
       </c>
@@ -3599,13 +4174,17 @@
         <v>48</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+      <c r="H113" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="I113" s="2"/>
+    </row>
+    <row r="114" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>299</v>
       </c>
@@ -3616,13 +4195,17 @@
         <v>48</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+      <c r="H114" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="I114" s="2"/>
+    </row>
+    <row r="115" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>301</v>
       </c>
@@ -3633,13 +4216,17 @@
         <v>48</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+      <c r="H115" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="I115" s="2"/>
+    </row>
+    <row r="116" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>303</v>
       </c>
@@ -3650,13 +4237,17 @@
         <v>48</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+      <c r="H116" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="I116" s="2"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>90</v>
       </c>
@@ -3669,8 +4260,12 @@
       <c r="F117" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H117" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I117" s="2"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>92</v>
       </c>
@@ -3683,8 +4278,12 @@
       <c r="F118" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H118" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I118" s="2"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>94</v>
       </c>
@@ -3697,8 +4296,12 @@
       <c r="F119" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H119" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I119" s="2"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>96</v>
       </c>
@@ -3711,8 +4314,12 @@
       <c r="F120" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H120" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I120" s="2"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>98</v>
       </c>
@@ -3725,8 +4332,12 @@
       <c r="F121" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H121" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I121" s="2"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>100</v>
       </c>
@@ -3739,8 +4350,12 @@
       <c r="F122" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H122" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I122" s="2"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>102</v>
       </c>
@@ -3753,20 +4368,28 @@
       <c r="F123" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H123" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I123" s="2"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H124" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I124" s="2"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Removed variables to be excluded due to poor skip pattern from data cleaning and codebook.
</commit_message>
<xml_diff>
--- a/codebooks/CSEC_Colombia_codebook.xlsx
+++ b/codebooks/CSEC_Colombia_codebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Isaac/Documents/2025_Colombia_CSEC/codebooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2025_Colombia_CSEC\codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6A78E1-0A50-224E-9302-3BAA03DAC237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4148D79A-4F30-4494-BA1D-554AD2D3D435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2480" yWindow="660" windowWidth="26160" windowHeight="17200" xr2:uid="{90244CBB-F4EA-4ADF-B7F8-E6030CEF41FB}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{90244CBB-F4EA-4ADF-B7F8-E6030CEF41FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="370">
   <si>
     <t>Variable</t>
   </si>
@@ -1162,6 +1162,15 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Excluded due to bad skip logic</t>
+  </si>
+  <si>
+    <t>Excluded due to scope</t>
   </si>
 </sst>
 </file>
@@ -1200,12 +1209,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.499984740745262"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1213,11 +1222,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalDown="1">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal style="thin">
+        <color auto="1"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1228,9 +1246,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1238,7 +1266,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1305,21 +1336,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3698636C-93CE-4425-935C-334B86A7B96E}" name="Table1" displayName="Table1" ref="A1:I124" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:I124" xr:uid="{3698636C-93CE-4425-935C-334B86A7B96E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3698636C-93CE-4425-935C-334B86A7B96E}" name="Table1" displayName="Table1" ref="A1:J124" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J124" xr:uid="{3698636C-93CE-4425-935C-334B86A7B96E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I124">
     <sortCondition ref="E1:E124"/>
   </sortState>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{2730ECEE-3C09-4BF5-890B-8860A9CFBE29}" name="Variable" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{1B48FA0F-CEB7-4E19-9CD2-A2270A8AEDC4}" name="VariableLabel" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{7642A26E-88CB-48B5-AECC-1FFA7324F1DD}" name="DataType" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{9DD7BF96-4287-49C0-901C-E4519D6003DE}" name="Questionnaire" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{BA0A682C-F3BF-499B-95BC-EB5277AFCFED}" name="RawNationalVar" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{1BA336CD-24B9-41F9-B139-898576B99FDF}" name="RawPriorityVar" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{9B023F9C-FAD5-4EB5-92F1-B039F8077C44}" name="Levels" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{2315BC48-3D3F-48E3-9101-8995A5E0E366}" name="Missing Status" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{905ED3C1-4347-4C3A-B678-A272BEEDEC6B}" name="Column1" dataDxfId="0"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{2730ECEE-3C09-4BF5-890B-8860A9CFBE29}" name="Variable" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{1B48FA0F-CEB7-4E19-9CD2-A2270A8AEDC4}" name="VariableLabel" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{7642A26E-88CB-48B5-AECC-1FFA7324F1DD}" name="DataType" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{9DD7BF96-4287-49C0-901C-E4519D6003DE}" name="Questionnaire" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{BA0A682C-F3BF-499B-95BC-EB5277AFCFED}" name="RawNationalVar" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{1BA336CD-24B9-41F9-B139-898576B99FDF}" name="RawPriorityVar" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{9B023F9C-FAD5-4EB5-92F1-B039F8077C44}" name="Levels" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{2315BC48-3D3F-48E3-9101-8995A5E0E366}" name="Missing Status" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{905ED3C1-4347-4C3A-B678-A272BEEDEC6B}" name="Column1" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{178899E5-8251-4246-BDD4-2332AD5C9628}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1642,25 +1674,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70025C6-7774-44FB-9A43-8696DD932E81}">
-  <dimension ref="A1:I134"/>
+  <dimension ref="A1:J134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="115" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L100" sqref="L100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="16" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5" style="2" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1688,8 +1721,11 @@
       <c r="I1" s="1" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J1" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>90</v>
       </c>
@@ -1706,8 +1742,9 @@
         <v>355</v>
       </c>
       <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -1735,8 +1772,9 @@
       <c r="I3" s="2" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -1764,8 +1802,9 @@
       <c r="I4" s="2" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1793,8 +1832,9 @@
       <c r="I5" s="2" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="365" x14ac:dyDescent="0.2">
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -1820,8 +1860,11 @@
         <v>357</v>
       </c>
       <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J6" s="9" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -1849,8 +1892,9 @@
       <c r="I7" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="132.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
@@ -1878,8 +1922,9 @@
       <c r="I8" s="2" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="144" x14ac:dyDescent="0.2">
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1907,8 +1952,9 @@
       <c r="I9" s="2" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -1936,8 +1982,9 @@
       <c r="I10" s="2" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -1965,8 +2012,9 @@
       <c r="I11" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -1994,8 +2042,9 @@
       <c r="I12" s="2" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -2023,8 +2072,9 @@
       <c r="I13" s="2" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>98</v>
       </c>
@@ -2041,8 +2091,9 @@
         <v>355</v>
       </c>
       <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>92</v>
       </c>
@@ -2059,8 +2110,9 @@
         <v>355</v>
       </c>
       <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>279</v>
       </c>
@@ -2080,8 +2132,9 @@
         <v>353</v>
       </c>
       <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>281</v>
       </c>
@@ -2101,8 +2154,9 @@
         <v>353</v>
       </c>
       <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>283</v>
       </c>
@@ -2122,8 +2176,9 @@
         <v>353</v>
       </c>
       <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>285</v>
       </c>
@@ -2143,8 +2198,9 @@
         <v>353</v>
       </c>
       <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>287</v>
       </c>
@@ -2164,8 +2220,9 @@
         <v>353</v>
       </c>
       <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>289</v>
       </c>
@@ -2185,8 +2242,9 @@
         <v>353</v>
       </c>
       <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>291</v>
       </c>
@@ -2206,8 +2264,9 @@
         <v>353</v>
       </c>
       <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>293</v>
       </c>
@@ -2227,8 +2286,9 @@
         <v>353</v>
       </c>
       <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>295</v>
       </c>
@@ -2248,8 +2308,9 @@
         <v>353</v>
       </c>
       <c r="I24" s="2"/>
-    </row>
-    <row r="25" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>297</v>
       </c>
@@ -2269,8 +2330,9 @@
         <v>353</v>
       </c>
       <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>299</v>
       </c>
@@ -2290,8 +2352,9 @@
         <v>353</v>
       </c>
       <c r="I26" s="2"/>
-    </row>
-    <row r="27" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>301</v>
       </c>
@@ -2311,8 +2374,9 @@
         <v>353</v>
       </c>
       <c r="I27" s="2"/>
-    </row>
-    <row r="28" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>303</v>
       </c>
@@ -2332,8 +2396,9 @@
         <v>353</v>
       </c>
       <c r="I28" s="2"/>
-    </row>
-    <row r="29" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>94</v>
       </c>
@@ -2350,8 +2415,9 @@
         <v>355</v>
       </c>
       <c r="I29" s="2"/>
-    </row>
-    <row r="30" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>201</v>
       </c>
@@ -2373,8 +2439,9 @@
       <c r="I30" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>203</v>
       </c>
@@ -2396,8 +2463,9 @@
       <c r="I31" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>205</v>
       </c>
@@ -2419,8 +2487,9 @@
       <c r="I32" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J32" s="2"/>
+    </row>
+    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>207</v>
       </c>
@@ -2442,8 +2511,9 @@
       <c r="I33" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J33" s="2"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>209</v>
       </c>
@@ -2463,8 +2533,9 @@
         <v>355</v>
       </c>
       <c r="I34" s="2"/>
-    </row>
-    <row r="35" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J34" s="2"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>211</v>
       </c>
@@ -2484,8 +2555,9 @@
         <v>355</v>
       </c>
       <c r="I35" s="2"/>
-    </row>
-    <row r="36" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J35" s="2"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>213</v>
       </c>
@@ -2505,8 +2577,9 @@
         <v>355</v>
       </c>
       <c r="I36" s="2"/>
-    </row>
-    <row r="37" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J36" s="2"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>215</v>
       </c>
@@ -2526,8 +2599,9 @@
         <v>355</v>
       </c>
       <c r="I37" s="2"/>
-    </row>
-    <row r="38" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J37" s="2"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>199</v>
       </c>
@@ -2547,8 +2621,9 @@
         <v>355</v>
       </c>
       <c r="I38" s="2"/>
-    </row>
-    <row r="39" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J38" s="2"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>189</v>
       </c>
@@ -2568,8 +2643,9 @@
         <v>355</v>
       </c>
       <c r="I39" s="2"/>
-    </row>
-    <row r="40" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J39" s="2"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>253</v>
       </c>
@@ -2589,8 +2665,9 @@
         <v>355</v>
       </c>
       <c r="I40" s="2"/>
-    </row>
-    <row r="41" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J40" s="2"/>
+    </row>
+    <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>255</v>
       </c>
@@ -2610,8 +2687,9 @@
         <v>355</v>
       </c>
       <c r="I41" s="2"/>
-    </row>
-    <row r="42" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J41" s="2"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>257</v>
       </c>
@@ -2631,8 +2709,9 @@
         <v>355</v>
       </c>
       <c r="I42" s="2"/>
-    </row>
-    <row r="43" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J42" s="2"/>
+    </row>
+    <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>259</v>
       </c>
@@ -2652,8 +2731,9 @@
         <v>355</v>
       </c>
       <c r="I43" s="2"/>
-    </row>
-    <row r="44" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J43" s="2"/>
+    </row>
+    <row r="44" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>261</v>
       </c>
@@ -2673,8 +2753,9 @@
         <v>355</v>
       </c>
       <c r="I44" s="2"/>
-    </row>
-    <row r="45" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J44" s="2"/>
+    </row>
+    <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>263</v>
       </c>
@@ -2694,8 +2775,9 @@
         <v>355</v>
       </c>
       <c r="I45" s="2"/>
-    </row>
-    <row r="46" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J45" s="2"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>191</v>
       </c>
@@ -2715,8 +2797,9 @@
         <v>355</v>
       </c>
       <c r="I46" s="2"/>
-    </row>
-    <row r="47" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J46" s="2"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>193</v>
       </c>
@@ -2736,8 +2819,9 @@
         <v>355</v>
       </c>
       <c r="I47" s="2"/>
-    </row>
-    <row r="48" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J47" s="2"/>
+    </row>
+    <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>195</v>
       </c>
@@ -2759,8 +2843,9 @@
       <c r="I48" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J48" s="2"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>197</v>
       </c>
@@ -2780,8 +2865,9 @@
         <v>355</v>
       </c>
       <c r="I49" s="2"/>
-    </row>
-    <row r="50" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J49" s="2"/>
+    </row>
+    <row r="50" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>217</v>
       </c>
@@ -2801,8 +2887,9 @@
         <v>355</v>
       </c>
       <c r="I50" s="2"/>
-    </row>
-    <row r="51" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J50" s="2"/>
+    </row>
+    <row r="51" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>219</v>
       </c>
@@ -2822,8 +2909,9 @@
         <v>355</v>
       </c>
       <c r="I51" s="2"/>
-    </row>
-    <row r="52" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J51" s="2"/>
+    </row>
+    <row r="52" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>221</v>
       </c>
@@ -2843,8 +2931,9 @@
         <v>355</v>
       </c>
       <c r="I52" s="2"/>
-    </row>
-    <row r="53" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J52" s="2"/>
+    </row>
+    <row r="53" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>223</v>
       </c>
@@ -2864,8 +2953,9 @@
         <v>355</v>
       </c>
       <c r="I53" s="2"/>
-    </row>
-    <row r="54" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J53" s="2"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>107</v>
       </c>
@@ -2885,8 +2975,9 @@
         <v>355</v>
       </c>
       <c r="I54" s="2"/>
-    </row>
-    <row r="55" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="J54" s="2"/>
+    </row>
+    <row r="55" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>225</v>
       </c>
@@ -2906,8 +2997,9 @@
         <v>355</v>
       </c>
       <c r="I55" s="2"/>
-    </row>
-    <row r="56" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="J55" s="2"/>
+    </row>
+    <row r="56" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>227</v>
       </c>
@@ -2927,8 +3019,9 @@
         <v>355</v>
       </c>
       <c r="I56" s="2"/>
-    </row>
-    <row r="57" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="J56" s="2"/>
+    </row>
+    <row r="57" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>229</v>
       </c>
@@ -2948,8 +3041,9 @@
         <v>355</v>
       </c>
       <c r="I57" s="2"/>
-    </row>
-    <row r="58" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="J57" s="2"/>
+    </row>
+    <row r="58" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>231</v>
       </c>
@@ -2969,8 +3063,9 @@
         <v>355</v>
       </c>
       <c r="I58" s="2"/>
-    </row>
-    <row r="59" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J58" s="2"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>109</v>
       </c>
@@ -2990,8 +3085,9 @@
         <v>355</v>
       </c>
       <c r="I59" s="2"/>
-    </row>
-    <row r="60" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J59" s="2"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>84</v>
       </c>
@@ -3014,8 +3110,9 @@
         <v>355</v>
       </c>
       <c r="I60" s="2"/>
-    </row>
-    <row r="61" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J60" s="2"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>121</v>
       </c>
@@ -3037,52 +3134,63 @@
       <c r="I61" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
+      <c r="J61" s="2"/>
+    </row>
+    <row r="62" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E62" s="2" t="s">
+      <c r="C62" s="6"/>
+      <c r="D62" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E62" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F62" s="2" t="s">
+      <c r="F62" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H62" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="I62" s="2" t="s">
+      <c r="G62" s="6"/>
+      <c r="H62" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="I62" s="6" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
+      <c r="J62" s="9" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="D63" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E63" s="2" t="s">
+      <c r="C63" s="6"/>
+      <c r="D63" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E63" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F63" s="2" t="s">
+      <c r="F63" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H63" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="I63" s="2"/>
-    </row>
-    <row r="64" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="G63" s="6"/>
+      <c r="H63" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="I63" s="6"/>
+      <c r="J63" s="9" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>111</v>
       </c>
@@ -3102,8 +3210,9 @@
         <v>355</v>
       </c>
       <c r="I64" s="2"/>
-    </row>
-    <row r="65" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J64" s="2"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>86</v>
       </c>
@@ -3123,8 +3232,9 @@
         <v>355</v>
       </c>
       <c r="I65" s="2"/>
-    </row>
-    <row r="66" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J65" s="2"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>88</v>
       </c>
@@ -3144,8 +3254,9 @@
         <v>355</v>
       </c>
       <c r="I66" s="2"/>
-    </row>
-    <row r="67" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J66" s="2"/>
+    </row>
+    <row r="67" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>233</v>
       </c>
@@ -3165,8 +3276,9 @@
         <v>355</v>
       </c>
       <c r="I67" s="2"/>
-    </row>
-    <row r="68" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J67" s="2"/>
+    </row>
+    <row r="68" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>235</v>
       </c>
@@ -3186,8 +3298,9 @@
         <v>355</v>
       </c>
       <c r="I68" s="2"/>
-    </row>
-    <row r="69" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J68" s="2"/>
+    </row>
+    <row r="69" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>237</v>
       </c>
@@ -3207,8 +3320,9 @@
         <v>355</v>
       </c>
       <c r="I69" s="2"/>
-    </row>
-    <row r="70" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J69" s="2"/>
+    </row>
+    <row r="70" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>239</v>
       </c>
@@ -3228,8 +3342,9 @@
         <v>355</v>
       </c>
       <c r="I70" s="2"/>
-    </row>
-    <row r="71" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J70" s="2"/>
+    </row>
+    <row r="71" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>241</v>
       </c>
@@ -3251,8 +3366,9 @@
       <c r="I71" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J71" s="2"/>
+    </row>
+    <row r="72" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>243</v>
       </c>
@@ -3274,8 +3390,9 @@
       <c r="I72" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J72" s="2"/>
+    </row>
+    <row r="73" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>245</v>
       </c>
@@ -3297,8 +3414,9 @@
       <c r="I73" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J73" s="2"/>
+    </row>
+    <row r="74" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>247</v>
       </c>
@@ -3320,8 +3438,9 @@
       <c r="I74" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J74" s="2"/>
+    </row>
+    <row r="75" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>249</v>
       </c>
@@ -3343,8 +3462,9 @@
       <c r="I75" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J75" s="2"/>
+    </row>
+    <row r="76" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>251</v>
       </c>
@@ -3366,31 +3486,37 @@
       <c r="I76" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
+      <c r="J76" s="2"/>
+    </row>
+    <row r="77" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A77" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E77" s="2" t="s">
+      <c r="C77" s="6"/>
+      <c r="D77" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E77" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F77" s="2" t="s">
+      <c r="F77" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H77" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="I77" s="2" t="s">
+      <c r="G77" s="6"/>
+      <c r="H77" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="I77" s="6" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J77" s="9" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>123</v>
       </c>
@@ -3412,228 +3538,279 @@
       <c r="I78" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
+      <c r="J78" s="2"/>
+    </row>
+    <row r="79" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A79" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E79" s="2" t="s">
+      <c r="C79" s="6"/>
+      <c r="D79" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E79" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="F79" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="H79" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="I79" s="2" t="s">
+      <c r="G79" s="6"/>
+      <c r="H79" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="I79" s="6" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
+      <c r="J79" s="9" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A80" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="D80" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E80" s="2" t="s">
+      <c r="C80" s="6"/>
+      <c r="D80" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E80" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F80" s="2" t="s">
+      <c r="F80" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="H80" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="I80" s="2"/>
-    </row>
-    <row r="81" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
+      <c r="G80" s="6"/>
+      <c r="H80" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="I80" s="6"/>
+      <c r="J80" s="9" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A81" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B81" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="D81" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E81" s="2" t="s">
+      <c r="C81" s="6"/>
+      <c r="D81" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E81" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="F81" s="2" t="s">
+      <c r="F81" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="H81" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="I81" s="2" t="s">
+      <c r="G81" s="6"/>
+      <c r="H81" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="I81" s="6" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
+      <c r="J81" s="9" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A82" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B82" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="D82" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E82" s="2" t="s">
+      <c r="C82" s="6"/>
+      <c r="D82" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E82" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="F82" s="2" t="s">
+      <c r="F82" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="H82" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="I82" s="2"/>
-    </row>
-    <row r="83" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
+      <c r="G82" s="6"/>
+      <c r="H82" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="I82" s="6"/>
+      <c r="J82" s="9" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A83" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B83" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="D83" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E83" s="2" t="s">
+      <c r="C83" s="6"/>
+      <c r="D83" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E83" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="F83" s="2" t="s">
+      <c r="F83" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="H83" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="I83" s="2" t="s">
+      <c r="G83" s="6"/>
+      <c r="H83" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="I83" s="6" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
+      <c r="J83" s="9" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A84" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B84" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="D84" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E84" s="2" t="s">
+      <c r="C84" s="6"/>
+      <c r="D84" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E84" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="F84" s="2" t="s">
+      <c r="F84" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="H84" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="I84" s="2"/>
-    </row>
-    <row r="85" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
+      <c r="G84" s="6"/>
+      <c r="H84" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="I84" s="6"/>
+      <c r="J84" s="9" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A85" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B85" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="D85" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E85" s="2" t="s">
+      <c r="C85" s="6"/>
+      <c r="D85" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E85" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="F85" s="2" t="s">
+      <c r="F85" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="H85" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="I85" s="2" t="s">
+      <c r="G85" s="6"/>
+      <c r="H85" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="I85" s="6" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
+      <c r="J85" s="9" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A86" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B86" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="D86" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E86" s="2" t="s">
+      <c r="C86" s="6"/>
+      <c r="D86" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E86" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="F86" s="2" t="s">
+      <c r="F86" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="H86" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="I86" s="2"/>
-    </row>
-    <row r="87" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
+      <c r="G86" s="6"/>
+      <c r="H86" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="I86" s="6"/>
+      <c r="J86" s="9" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A87" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B87" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="D87" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E87" s="2" t="s">
+      <c r="C87" s="6"/>
+      <c r="D87" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E87" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="F87" s="2" t="s">
+      <c r="F87" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="H87" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="I87" s="2" t="s">
+      <c r="G87" s="6"/>
+      <c r="H87" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="I87" s="6" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
+      <c r="J87" s="9" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A88" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B88" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="D88" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E88" s="2" t="s">
+      <c r="C88" s="6"/>
+      <c r="D88" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E88" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="F88" s="2" t="s">
+      <c r="F88" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="H88" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="I88" s="2"/>
-    </row>
-    <row r="89" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="G88" s="6"/>
+      <c r="H88" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="I88" s="6"/>
+      <c r="J88" s="9" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>151</v>
       </c>
@@ -3655,8 +3832,9 @@
       <c r="I89" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J89" s="2"/>
+    </row>
+    <row r="90" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>161</v>
       </c>
@@ -3676,8 +3854,9 @@
         <v>355</v>
       </c>
       <c r="I90" s="2"/>
-    </row>
-    <row r="91" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J90" s="2"/>
+    </row>
+    <row r="91" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>265</v>
       </c>
@@ -3699,8 +3878,9 @@
       <c r="I91" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J91" s="2"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>173</v>
       </c>
@@ -3720,31 +3900,37 @@
         <v>355</v>
       </c>
       <c r="I92" s="2"/>
-    </row>
-    <row r="93" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A93" s="1" t="s">
+      <c r="J92" s="2"/>
+    </row>
+    <row r="93" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A93" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B93" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="D93" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E93" s="2" t="s">
+      <c r="C93" s="6"/>
+      <c r="D93" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E93" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="F93" s="2" t="s">
+      <c r="F93" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="H93" s="2" t="s">
+      <c r="G93" s="6"/>
+      <c r="H93" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="I93" s="2" t="s">
+      <c r="I93" s="6" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J93" s="9" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>175</v>
       </c>
@@ -3766,8 +3952,9 @@
       <c r="I94" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J94" s="2"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>269</v>
       </c>
@@ -3789,8 +3976,9 @@
       <c r="I95" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J95" s="2"/>
+    </row>
+    <row r="96" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>177</v>
       </c>
@@ -3812,8 +4000,9 @@
       <c r="I96" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J96" s="2"/>
+    </row>
+    <row r="97" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>275</v>
       </c>
@@ -3833,75 +4022,91 @@
         <v>363</v>
       </c>
       <c r="I97" s="2"/>
-    </row>
-    <row r="98" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A98" s="1" t="s">
+      <c r="J97" s="2"/>
+    </row>
+    <row r="98" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A98" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B98" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="D98" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E98" s="2" t="s">
+      <c r="C98" s="6"/>
+      <c r="D98" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E98" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="F98" s="2" t="s">
+      <c r="F98" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="H98" s="2" t="s">
+      <c r="G98" s="6"/>
+      <c r="H98" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="I98" s="2"/>
-    </row>
-    <row r="99" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A99" s="1" t="s">
+      <c r="I98" s="6"/>
+      <c r="J98" s="9" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A99" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B99" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="D99" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E99" s="2" t="s">
+      <c r="C99" s="6"/>
+      <c r="D99" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E99" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F99" s="2" t="s">
+      <c r="F99" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="H99" s="2" t="s">
+      <c r="G99" s="6"/>
+      <c r="H99" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="I99" s="2" t="s">
+      <c r="I99" s="6" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A100" s="1" t="s">
+      <c r="J99" s="9" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A100" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B100" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="D100" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E100" s="2" t="s">
+      <c r="C100" s="6"/>
+      <c r="D100" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E100" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F100" s="2" t="s">
+      <c r="F100" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H100" s="2" t="s">
+      <c r="G100" s="6"/>
+      <c r="H100" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="I100" s="2" t="s">
+      <c r="I100" s="6" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J100" s="9" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>113</v>
       </c>
@@ -3923,8 +4128,9 @@
       <c r="I101" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J101" s="2"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>163</v>
       </c>
@@ -3944,8 +4150,9 @@
         <v>355</v>
       </c>
       <c r="I102" s="2"/>
-    </row>
-    <row r="103" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J102" s="2"/>
+    </row>
+    <row r="103" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>179</v>
       </c>
@@ -3965,8 +4172,9 @@
         <v>355</v>
       </c>
       <c r="I103" s="2"/>
-    </row>
-    <row r="104" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J103" s="2"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>125</v>
       </c>
@@ -3986,8 +4194,9 @@
         <v>355</v>
       </c>
       <c r="I104" s="2"/>
-    </row>
-    <row r="105" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J104" s="2"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>127</v>
       </c>
@@ -4007,8 +4216,9 @@
         <v>355</v>
       </c>
       <c r="I105" s="2"/>
-    </row>
-    <row r="106" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J105" s="2"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>115</v>
       </c>
@@ -4028,8 +4238,9 @@
         <v>355</v>
       </c>
       <c r="I106" s="2"/>
-    </row>
-    <row r="107" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J106" s="2"/>
+    </row>
+    <row r="107" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>181</v>
       </c>
@@ -4049,8 +4260,9 @@
         <v>355</v>
       </c>
       <c r="I107" s="2"/>
-    </row>
-    <row r="108" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J107" s="2"/>
+    </row>
+    <row r="108" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>183</v>
       </c>
@@ -4070,8 +4282,9 @@
         <v>355</v>
       </c>
       <c r="I108" s="2"/>
-    </row>
-    <row r="109" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J108" s="2"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>117</v>
       </c>
@@ -4091,100 +4304,121 @@
         <v>355</v>
       </c>
       <c r="I109" s="2"/>
-    </row>
-    <row r="110" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A110" s="1" t="s">
+      <c r="J109" s="2"/>
+    </row>
+    <row r="110" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A110" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="D110" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E110" s="2" t="s">
+      <c r="C110" s="6"/>
+      <c r="D110" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E110" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="F110" s="2" t="s">
+      <c r="F110" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="H110" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="I110" s="2" t="s">
+      <c r="G110" s="6"/>
+      <c r="H110" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="I110" s="6" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A111" s="1" t="s">
+      <c r="J110" s="9" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A111" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="D111" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E111" s="2" t="s">
+      <c r="C111" s="6"/>
+      <c r="D111" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E111" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="F111" s="2" t="s">
+      <c r="F111" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="H111" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="I111" s="2" t="s">
+      <c r="G111" s="6"/>
+      <c r="H111" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="I111" s="6" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A112" s="1" t="s">
+      <c r="J111" s="9" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A112" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B112" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="D112" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E112" s="2" t="s">
+      <c r="C112" s="6"/>
+      <c r="D112" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E112" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="F112" s="2" t="s">
+      <c r="F112" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="H112" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="I112" s="2" t="s">
+      <c r="G112" s="6"/>
+      <c r="H112" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="I112" s="6" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A113" s="1" t="s">
+      <c r="J112" s="9" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A113" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B113" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="D113" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E113" s="2" t="s">
+      <c r="C113" s="6"/>
+      <c r="D113" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E113" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="F113" s="2" t="s">
+      <c r="F113" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="H113" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="I113" s="2" t="s">
+      <c r="G113" s="6"/>
+      <c r="H113" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="I113" s="6" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J113" s="9" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>165</v>
       </c>
@@ -4204,8 +4438,9 @@
         <v>355</v>
       </c>
       <c r="I114" s="2"/>
-    </row>
-    <row r="115" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J114" s="2"/>
+    </row>
+    <row r="115" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>185</v>
       </c>
@@ -4225,8 +4460,9 @@
         <v>355</v>
       </c>
       <c r="I115" s="2"/>
-    </row>
-    <row r="116" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J115" s="2"/>
+    </row>
+    <row r="116" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>187</v>
       </c>
@@ -4246,8 +4482,9 @@
         <v>355</v>
       </c>
       <c r="I116" s="2"/>
-    </row>
-    <row r="117" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J116" s="2"/>
+    </row>
+    <row r="117" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>167</v>
       </c>
@@ -4267,8 +4504,9 @@
         <v>362</v>
       </c>
       <c r="I117" s="2"/>
-    </row>
-    <row r="118" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J117" s="2"/>
+    </row>
+    <row r="118" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>169</v>
       </c>
@@ -4288,8 +4526,9 @@
         <v>362</v>
       </c>
       <c r="I118" s="2"/>
-    </row>
-    <row r="119" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J118" s="2"/>
+    </row>
+    <row r="119" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>171</v>
       </c>
@@ -4309,8 +4548,9 @@
         <v>362</v>
       </c>
       <c r="I119" s="2"/>
-    </row>
-    <row r="120" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J119" s="2"/>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>82</v>
       </c>
@@ -4333,8 +4573,9 @@
         <v>355</v>
       </c>
       <c r="I120" s="2"/>
-    </row>
-    <row r="121" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J120" s="2"/>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>96</v>
       </c>
@@ -4351,8 +4592,9 @@
         <v>355</v>
       </c>
       <c r="I121" s="2"/>
-    </row>
-    <row r="122" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J121" s="2"/>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>100</v>
       </c>
@@ -4369,8 +4611,9 @@
         <v>355</v>
       </c>
       <c r="I122" s="2"/>
-    </row>
-    <row r="123" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J122" s="2"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>102</v>
       </c>
@@ -4387,42 +4630,44 @@
         <v>355</v>
       </c>
       <c r="I123" s="2"/>
-    </row>
-    <row r="124" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J123" s="2"/>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="H124" s="2" t="s">
         <v>355</v>
       </c>
       <c r="I124" s="2"/>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J124" s="2"/>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
     </row>
   </sheetData>
@@ -4439,16 +4684,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC73D769-F89C-4778-8F24-4D313214FE79}">
   <dimension ref="A1:B122"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B122"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>82</v>
       </c>
@@ -4456,7 +4701,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -4464,7 +4709,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -4472,7 +4717,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -4480,7 +4725,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>90</v>
       </c>
@@ -4488,7 +4733,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>92</v>
       </c>
@@ -4496,7 +4741,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>94</v>
       </c>
@@ -4504,7 +4749,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>96</v>
       </c>
@@ -4512,7 +4757,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>98</v>
       </c>
@@ -4520,7 +4765,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>100</v>
       </c>
@@ -4528,7 +4773,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>102</v>
       </c>
@@ -4536,7 +4781,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -4544,7 +4789,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -4552,7 +4797,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -4560,7 +4805,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -4568,7 +4813,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -4576,7 +4821,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -4584,7 +4829,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -4592,7 +4837,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -4600,7 +4845,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -4608,7 +4853,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -4616,7 +4861,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -4624,7 +4869,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>105</v>
       </c>
@@ -4632,7 +4877,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>107</v>
       </c>
@@ -4640,7 +4885,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>109</v>
       </c>
@@ -4648,7 +4893,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>111</v>
       </c>
@@ -4656,7 +4901,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>113</v>
       </c>
@@ -4664,7 +4909,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>115</v>
       </c>
@@ -4672,7 +4917,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>117</v>
       </c>
@@ -4680,7 +4925,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>119</v>
       </c>
@@ -4688,7 +4933,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>121</v>
       </c>
@@ -4696,7 +4941,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>123</v>
       </c>
@@ -4704,7 +4949,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>125</v>
       </c>
@@ -4712,7 +4957,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>127</v>
       </c>
@@ -4720,7 +4965,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>129</v>
       </c>
@@ -4728,7 +4973,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>131</v>
       </c>
@@ -4736,7 +4981,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>133</v>
       </c>
@@ -4744,7 +4989,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>135</v>
       </c>
@@ -4752,7 +4997,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>137</v>
       </c>
@@ -4760,7 +5005,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>139</v>
       </c>
@@ -4768,7 +5013,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>141</v>
       </c>
@@ -4776,7 +5021,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>143</v>
       </c>
@@ -4784,7 +5029,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>145</v>
       </c>
@@ -4792,7 +5037,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>147</v>
       </c>
@@ -4800,7 +5045,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>149</v>
       </c>
@@ -4808,7 +5053,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>151</v>
       </c>
@@ -4816,7 +5061,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>153</v>
       </c>
@@ -4824,7 +5069,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>155</v>
       </c>
@@ -4832,7 +5077,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>157</v>
       </c>
@@ -4840,7 +5085,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>159</v>
       </c>
@@ -4848,7 +5093,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>161</v>
       </c>
@@ -4856,7 +5101,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>163</v>
       </c>
@@ -4864,7 +5109,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>165</v>
       </c>
@@ -4872,7 +5117,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>167</v>
       </c>
@@ -4880,7 +5125,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>169</v>
       </c>
@@ -4888,7 +5133,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>171</v>
       </c>
@@ -4896,7 +5141,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>173</v>
       </c>
@@ -4904,7 +5149,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>175</v>
       </c>
@@ -4912,7 +5157,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>177</v>
       </c>
@@ -4920,7 +5165,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>179</v>
       </c>
@@ -4928,7 +5173,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>181</v>
       </c>
@@ -4936,7 +5181,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>183</v>
       </c>
@@ -4944,7 +5189,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>185</v>
       </c>
@@ -4952,7 +5197,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>187</v>
       </c>
@@ -4960,7 +5205,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>189</v>
       </c>
@@ -4968,7 +5213,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>191</v>
       </c>
@@ -4976,7 +5221,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>193</v>
       </c>
@@ -4984,7 +5229,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>195</v>
       </c>
@@ -4992,7 +5237,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>197</v>
       </c>
@@ -5000,7 +5245,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>199</v>
       </c>
@@ -5008,7 +5253,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>201</v>
       </c>
@@ -5016,7 +5261,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>203</v>
       </c>
@@ -5024,7 +5269,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>205</v>
       </c>
@@ -5032,7 +5277,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>207</v>
       </c>
@@ -5040,7 +5285,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>209</v>
       </c>
@@ -5048,7 +5293,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>211</v>
       </c>
@@ -5056,7 +5301,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>213</v>
       </c>
@@ -5064,7 +5309,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>215</v>
       </c>
@@ -5072,7 +5317,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>217</v>
       </c>
@@ -5080,7 +5325,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>219</v>
       </c>
@@ -5088,7 +5333,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>221</v>
       </c>
@@ -5096,7 +5341,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>223</v>
       </c>
@@ -5104,7 +5349,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>225</v>
       </c>
@@ -5112,7 +5357,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>227</v>
       </c>
@@ -5120,7 +5365,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>229</v>
       </c>
@@ -5128,7 +5373,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>231</v>
       </c>
@@ -5136,7 +5381,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>233</v>
       </c>
@@ -5144,7 +5389,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>235</v>
       </c>
@@ -5152,7 +5397,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>237</v>
       </c>
@@ -5160,7 +5405,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>239</v>
       </c>
@@ -5168,7 +5413,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>241</v>
       </c>
@@ -5176,7 +5421,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>243</v>
       </c>
@@ -5184,7 +5429,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>245</v>
       </c>
@@ -5192,7 +5437,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>247</v>
       </c>
@@ -5200,7 +5445,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>249</v>
       </c>
@@ -5208,7 +5453,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>251</v>
       </c>
@@ -5216,7 +5461,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>253</v>
       </c>
@@ -5224,7 +5469,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>255</v>
       </c>
@@ -5232,7 +5477,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>257</v>
       </c>
@@ -5240,7 +5485,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>259</v>
       </c>
@@ -5248,7 +5493,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>261</v>
       </c>
@@ -5256,7 +5501,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>263</v>
       </c>
@@ -5264,7 +5509,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>265</v>
       </c>
@@ -5272,7 +5517,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>267</v>
       </c>
@@ -5280,7 +5525,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>269</v>
       </c>
@@ -5288,7 +5533,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>271</v>
       </c>
@@ -5296,7 +5541,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>273</v>
       </c>
@@ -5304,7 +5549,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>275</v>
       </c>
@@ -5312,7 +5557,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>277</v>
       </c>
@@ -5320,7 +5565,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>279</v>
       </c>
@@ -5328,7 +5573,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>281</v>
       </c>
@@ -5336,7 +5581,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>283</v>
       </c>
@@ -5344,7 +5589,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>285</v>
       </c>
@@ -5352,7 +5597,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>287</v>
       </c>
@@ -5360,7 +5605,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>289</v>
       </c>
@@ -5368,7 +5613,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>291</v>
       </c>
@@ -5376,7 +5621,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>293</v>
       </c>
@@ -5384,7 +5629,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>295</v>
       </c>
@@ -5392,7 +5637,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>297</v>
       </c>
@@ -5400,7 +5645,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>299</v>
       </c>
@@ -5408,7 +5653,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>301</v>
       </c>
@@ -5416,7 +5661,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>303</v>
       </c>
@@ -5437,7 +5682,7 @@
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>